<commit_message>
adicionando preenchimento de estatíticas
</commit_message>
<xml_diff>
--- a/Modelo DRAA Precificador.xlsx
+++ b/Modelo DRAA Precificador.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/395120fd4aa672be/Compartilhados/Wuisley-INOVE/Python/plano de amortização/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wuisl\Documents\Python\plano de amortização\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87AA7F52-4E03-49E7-83B5-1F359BDE8EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C78692-EE13-4E5C-A679-35B68245A5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="28800" windowHeight="11385" xr2:uid="{87BBCD0E-C408-44A6-9AEE-4B69C2883792}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{87BBCD0E-C408-44A6-9AEE-4B69C2883792}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$5:$M$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$5:$N$15</definedName>
     <definedName name="sel_orgaos">Planilha1!$C$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="25">
   <si>
     <t>Número Critério</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Assembleia</t>
+  </si>
+  <si>
+    <t>COD_TIPO</t>
   </si>
 </sst>
 </file>
@@ -147,7 +150,7 @@
       <name val="Maven Pro"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +166,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -344,7 +359,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -392,6 +407,28 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -830,22 +867,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{096FA669-5DD0-4A13-82FB-E3FC1F8A4970}">
-  <dimension ref="A5:M25"/>
+  <dimension ref="A5:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="J24" sqref="J24:N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -859,38 +897,41 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="18">
         <v>3</v>
       </c>
       <c r="C6" s="2">
@@ -899,39 +940,42 @@
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="14" t="s">
+      <c r="E6" s="17">
+        <v>1</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="5">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0</v>
-      </c>
-      <c r="K6" s="6">
-        <v>0</v>
-      </c>
-      <c r="L6" s="6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="19">
+        <v>0</v>
+      </c>
+      <c r="K6" s="20">
+        <v>0</v>
+      </c>
+      <c r="L6" s="20">
+        <v>0</v>
+      </c>
+      <c r="M6" s="20">
+        <v>0</v>
+      </c>
+      <c r="N6" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="18">
         <v>3</v>
       </c>
       <c r="C7" s="2">
@@ -940,40 +984,43 @@
       <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="15" t="str">
-        <f>F6</f>
+      <c r="E7" s="17">
+        <v>1</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="15" t="str">
+        <f>G6</f>
         <v>MAGISTRADO</v>
       </c>
-      <c r="G7" s="8">
-        <v>1</v>
-      </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="10">
-        <v>0</v>
-      </c>
-      <c r="J7" s="11">
-        <v>0</v>
-      </c>
-      <c r="K7" s="11">
-        <v>0</v>
-      </c>
-      <c r="L7" s="11">
-        <v>0</v>
-      </c>
-      <c r="M7" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J7" s="22">
+        <v>0</v>
+      </c>
+      <c r="K7" s="23">
+        <v>0</v>
+      </c>
+      <c r="L7" s="23">
+        <v>0</v>
+      </c>
+      <c r="M7" s="23">
+        <v>0</v>
+      </c>
+      <c r="N7" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="18">
         <v>3</v>
       </c>
       <c r="C8" s="2">
@@ -982,39 +1029,42 @@
       <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="14" t="s">
+      <c r="E8" s="17">
+        <v>1</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <v>2</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="5">
-        <v>0</v>
-      </c>
-      <c r="J8" s="6">
-        <v>0</v>
-      </c>
-      <c r="K8" s="6">
-        <v>0</v>
-      </c>
-      <c r="L8" s="6">
-        <v>0</v>
-      </c>
-      <c r="M8" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J8" s="19">
+        <v>0</v>
+      </c>
+      <c r="K8" s="20">
+        <v>0</v>
+      </c>
+      <c r="L8" s="20">
+        <v>0</v>
+      </c>
+      <c r="M8" s="20">
+        <v>0</v>
+      </c>
+      <c r="N8" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="18">
         <v>3</v>
       </c>
       <c r="C9" s="2">
@@ -1023,40 +1073,43 @@
       <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="15" t="str">
-        <f>F8</f>
+      <c r="E9" s="17">
+        <v>1</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="15" t="str">
+        <f>G8</f>
         <v>PROF</v>
       </c>
-      <c r="G9" s="8">
+      <c r="H9" s="8">
         <v>2</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="I9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="10">
-        <v>0</v>
-      </c>
-      <c r="J9" s="11">
-        <v>0</v>
-      </c>
-      <c r="K9" s="11">
-        <v>0</v>
-      </c>
-      <c r="L9" s="11">
-        <v>0</v>
-      </c>
-      <c r="M9" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="22">
+        <v>0</v>
+      </c>
+      <c r="K9" s="23">
+        <v>0</v>
+      </c>
+      <c r="L9" s="23">
+        <v>0</v>
+      </c>
+      <c r="M9" s="23">
+        <v>0</v>
+      </c>
+      <c r="N9" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="18">
         <v>3</v>
       </c>
       <c r="C10" s="2">
@@ -1065,39 +1118,42 @@
       <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="14" t="s">
+      <c r="E10" s="17">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>3</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="5">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6">
-        <v>0</v>
-      </c>
-      <c r="K10" s="6">
-        <v>0</v>
-      </c>
-      <c r="L10" s="6">
-        <v>0</v>
-      </c>
-      <c r="M10" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J10" s="19">
+        <v>0</v>
+      </c>
+      <c r="K10" s="20">
+        <v>0</v>
+      </c>
+      <c r="L10" s="20">
+        <v>0</v>
+      </c>
+      <c r="M10" s="20">
+        <v>0</v>
+      </c>
+      <c r="N10" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="18">
         <v>3</v>
       </c>
       <c r="C11" s="2">
@@ -1106,40 +1162,43 @@
       <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="15" t="str">
-        <f>F10</f>
+      <c r="E11" s="17">
+        <v>1</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="15" t="str">
+        <f>G10</f>
         <v>MILITAR</v>
       </c>
-      <c r="G11" s="8">
+      <c r="H11" s="8">
         <v>3</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="I11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="10">
-        <v>0</v>
-      </c>
-      <c r="J11" s="11">
-        <v>0</v>
-      </c>
-      <c r="K11" s="11">
-        <v>0</v>
-      </c>
-      <c r="L11" s="11">
-        <v>0</v>
-      </c>
-      <c r="M11" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J11" s="22">
+        <v>0</v>
+      </c>
+      <c r="K11" s="23">
+        <v>0</v>
+      </c>
+      <c r="L11" s="23">
+        <v>0</v>
+      </c>
+      <c r="M11" s="23">
+        <v>0</v>
+      </c>
+      <c r="N11" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="18">
         <v>3</v>
       </c>
       <c r="C12" s="2">
@@ -1148,39 +1207,42 @@
       <c r="D12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="16" t="s">
+      <c r="E12" s="17">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="3">
         <v>4</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="5">
+      <c r="J12" s="5">
         <v>10</v>
       </c>
-      <c r="J12" s="6">
+      <c r="K12" s="6">
         <v>409151</v>
       </c>
-      <c r="K12" s="6">
+      <c r="L12" s="6">
         <v>3610</v>
       </c>
-      <c r="L12" s="6">
+      <c r="M12" s="6">
         <v>6000</v>
       </c>
-      <c r="M12" s="7">
+      <c r="N12" s="7">
         <v>2680</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="18">
         <v>3</v>
       </c>
       <c r="C13" s="2">
@@ -1189,40 +1251,43 @@
       <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="15" t="str">
-        <f>F12</f>
+      <c r="E13" s="17">
+        <v>1</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="15" t="str">
+        <f>G12</f>
         <v>OUTROS</v>
       </c>
-      <c r="G13" s="8">
+      <c r="H13" s="8">
         <v>4</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="I13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="10">
-        <v>12</v>
-      </c>
-      <c r="J13" s="11">
+      <c r="J13" s="10">
+        <v>12</v>
+      </c>
+      <c r="K13" s="11">
         <v>346347.08333333331</v>
       </c>
-      <c r="K13" s="11">
+      <c r="L13" s="11">
         <v>3941.6666666666665</v>
       </c>
-      <c r="L13" s="11">
+      <c r="M13" s="11">
         <v>5533.3333333333339</v>
       </c>
-      <c r="M13" s="12">
+      <c r="N13" s="12">
         <v>3083.333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="18">
         <v>3</v>
       </c>
       <c r="C14" s="2">
@@ -1231,39 +1296,42 @@
       <c r="D14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="14" t="s">
+      <c r="E14" s="17">
+        <v>1</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="3">
+      <c r="H14" s="3">
         <v>5</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="5">
-        <v>0</v>
-      </c>
-      <c r="J14" s="6">
-        <v>0</v>
-      </c>
-      <c r="K14" s="6">
-        <v>0</v>
-      </c>
-      <c r="L14" s="6">
-        <v>0</v>
-      </c>
-      <c r="M14" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J14" s="19">
+        <v>0</v>
+      </c>
+      <c r="K14" s="20">
+        <v>0</v>
+      </c>
+      <c r="L14" s="20">
+        <v>0</v>
+      </c>
+      <c r="M14" s="20">
+        <v>0</v>
+      </c>
+      <c r="N14" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="18">
         <v>3</v>
       </c>
       <c r="C15" s="2">
@@ -1272,40 +1340,43 @@
       <c r="D15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="15" t="str">
-        <f>F14</f>
+      <c r="E15" s="17">
+        <v>1</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="15" t="str">
+        <f>G14</f>
         <v>PROF SUP</v>
       </c>
-      <c r="G15" s="8">
+      <c r="H15" s="8">
         <v>5</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="I15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="10">
-        <v>0</v>
-      </c>
-      <c r="J15" s="11">
-        <v>0</v>
-      </c>
-      <c r="K15" s="11">
-        <v>0</v>
-      </c>
-      <c r="L15" s="11">
-        <v>0</v>
-      </c>
-      <c r="M15" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J15" s="22">
+        <v>0</v>
+      </c>
+      <c r="K15" s="23">
+        <v>0</v>
+      </c>
+      <c r="L15" s="23">
+        <v>0</v>
+      </c>
+      <c r="M15" s="23">
+        <v>0</v>
+      </c>
+      <c r="N15" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="18">
         <v>4</v>
       </c>
       <c r="C16" s="2">
@@ -1314,39 +1385,42 @@
       <c r="D16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="14" t="s">
+      <c r="E16" s="17">
+        <v>1</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="3">
-        <v>1</v>
-      </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="5">
-        <v>0</v>
-      </c>
-      <c r="J16" s="6">
-        <v>0</v>
-      </c>
-      <c r="K16" s="6">
-        <v>0</v>
-      </c>
-      <c r="L16" s="6">
-        <v>0</v>
-      </c>
-      <c r="M16" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J16" s="19">
+        <v>0</v>
+      </c>
+      <c r="K16" s="20">
+        <v>0</v>
+      </c>
+      <c r="L16" s="20">
+        <v>0</v>
+      </c>
+      <c r="M16" s="20">
+        <v>0</v>
+      </c>
+      <c r="N16" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="18">
         <v>4</v>
       </c>
       <c r="C17" s="2">
@@ -1355,40 +1429,43 @@
       <c r="D17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="15" t="str">
-        <f>F16</f>
+      <c r="E17" s="17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="15" t="str">
+        <f>G16</f>
         <v>MAGISTRADO</v>
       </c>
-      <c r="G17" s="8">
-        <v>1</v>
-      </c>
-      <c r="H17" s="9" t="s">
+      <c r="H17" s="8">
+        <v>1</v>
+      </c>
+      <c r="I17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="10">
-        <v>0</v>
-      </c>
-      <c r="J17" s="11">
-        <v>0</v>
-      </c>
-      <c r="K17" s="11">
-        <v>0</v>
-      </c>
-      <c r="L17" s="11">
-        <v>0</v>
-      </c>
-      <c r="M17" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J17" s="22">
+        <v>0</v>
+      </c>
+      <c r="K17" s="23">
+        <v>0</v>
+      </c>
+      <c r="L17" s="23">
+        <v>0</v>
+      </c>
+      <c r="M17" s="23">
+        <v>0</v>
+      </c>
+      <c r="N17" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="18">
         <v>4</v>
       </c>
       <c r="C18" s="2">
@@ -1397,39 +1474,42 @@
       <c r="D18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="14" t="s">
+      <c r="E18" s="17">
+        <v>1</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="3">
+      <c r="H18" s="3">
         <v>2</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="I18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I18" s="5">
-        <v>0</v>
-      </c>
-      <c r="J18" s="6">
-        <v>0</v>
-      </c>
-      <c r="K18" s="6">
-        <v>0</v>
-      </c>
-      <c r="L18" s="6">
-        <v>0</v>
-      </c>
-      <c r="M18" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="19">
+        <v>0</v>
+      </c>
+      <c r="K18" s="20">
+        <v>0</v>
+      </c>
+      <c r="L18" s="20">
+        <v>0</v>
+      </c>
+      <c r="M18" s="20">
+        <v>0</v>
+      </c>
+      <c r="N18" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="18">
         <v>4</v>
       </c>
       <c r="C19" s="2">
@@ -1438,40 +1518,43 @@
       <c r="D19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="15" t="str">
-        <f>F18</f>
+      <c r="E19" s="17">
+        <v>1</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="15" t="str">
+        <f>G18</f>
         <v>PROF</v>
       </c>
-      <c r="G19" s="8">
+      <c r="H19" s="8">
         <v>2</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="I19" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="10">
-        <v>0</v>
-      </c>
-      <c r="J19" s="11">
-        <v>0</v>
-      </c>
-      <c r="K19" s="11">
-        <v>0</v>
-      </c>
-      <c r="L19" s="11">
-        <v>0</v>
-      </c>
-      <c r="M19" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J19" s="22">
+        <v>0</v>
+      </c>
+      <c r="K19" s="23">
+        <v>0</v>
+      </c>
+      <c r="L19" s="23">
+        <v>0</v>
+      </c>
+      <c r="M19" s="23">
+        <v>0</v>
+      </c>
+      <c r="N19" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="18">
         <v>4</v>
       </c>
       <c r="C20" s="2">
@@ -1480,39 +1563,42 @@
       <c r="D20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="14" t="s">
+      <c r="E20" s="17">
+        <v>1</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="3">
+      <c r="H20" s="3">
         <v>3</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="I20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="5">
-        <v>0</v>
-      </c>
-      <c r="J20" s="6">
-        <v>0</v>
-      </c>
-      <c r="K20" s="6">
-        <v>0</v>
-      </c>
-      <c r="L20" s="6">
-        <v>0</v>
-      </c>
-      <c r="M20" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J20" s="19">
+        <v>0</v>
+      </c>
+      <c r="K20" s="20">
+        <v>0</v>
+      </c>
+      <c r="L20" s="20">
+        <v>0</v>
+      </c>
+      <c r="M20" s="20">
+        <v>0</v>
+      </c>
+      <c r="N20" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="18">
         <v>4</v>
       </c>
       <c r="C21" s="2">
@@ -1521,40 +1607,43 @@
       <c r="D21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="15" t="str">
-        <f>F20</f>
+      <c r="E21" s="17">
+        <v>1</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="15" t="str">
+        <f>G20</f>
         <v>MILITAR</v>
       </c>
-      <c r="G21" s="8">
+      <c r="H21" s="8">
         <v>3</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="I21" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I21" s="10">
-        <v>0</v>
-      </c>
-      <c r="J21" s="11">
-        <v>0</v>
-      </c>
-      <c r="K21" s="11">
-        <v>0</v>
-      </c>
-      <c r="L21" s="11">
-        <v>0</v>
-      </c>
-      <c r="M21" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J21" s="22">
+        <v>0</v>
+      </c>
+      <c r="K21" s="23">
+        <v>0</v>
+      </c>
+      <c r="L21" s="23">
+        <v>0</v>
+      </c>
+      <c r="M21" s="23">
+        <v>0</v>
+      </c>
+      <c r="N21" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="18">
         <v>4</v>
       </c>
       <c r="C22" s="2">
@@ -1563,39 +1652,42 @@
       <c r="D22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="16" t="s">
+      <c r="E22" s="17">
+        <v>1</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="3">
+      <c r="H22" s="3">
         <v>4</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="I22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="5">
+      <c r="J22" s="5">
         <v>10</v>
       </c>
-      <c r="J22" s="6">
+      <c r="K22" s="6">
         <v>409151</v>
       </c>
-      <c r="K22" s="6">
+      <c r="L22" s="6">
         <v>3610</v>
       </c>
-      <c r="L22" s="6">
+      <c r="M22" s="6">
         <v>6000</v>
       </c>
-      <c r="M22" s="7">
+      <c r="N22" s="7">
         <v>2680</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="18">
         <v>4</v>
       </c>
       <c r="C23" s="2">
@@ -1604,40 +1696,43 @@
       <c r="D23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="15" t="str">
-        <f>F22</f>
+      <c r="E23" s="17">
+        <v>1</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="15" t="str">
+        <f>G22</f>
         <v>OUTROS</v>
       </c>
-      <c r="G23" s="8">
+      <c r="H23" s="8">
         <v>4</v>
       </c>
-      <c r="H23" s="9" t="s">
+      <c r="I23" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I23" s="10">
-        <v>12</v>
-      </c>
-      <c r="J23" s="11">
+      <c r="J23" s="10">
+        <v>12</v>
+      </c>
+      <c r="K23" s="11">
         <v>346347.08333333331</v>
       </c>
-      <c r="K23" s="11">
+      <c r="L23" s="11">
         <v>3941.6666666666665</v>
       </c>
-      <c r="L23" s="11">
+      <c r="M23" s="11">
         <v>5533.3333333333339</v>
       </c>
-      <c r="M23" s="12">
+      <c r="N23" s="12">
         <v>3083.333333333333</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="18">
         <v>4</v>
       </c>
       <c r="C24" s="2">
@@ -1646,39 +1741,42 @@
       <c r="D24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="14" t="s">
+      <c r="E24" s="17">
+        <v>1</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="3">
+      <c r="H24" s="3">
         <v>5</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="I24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I24" s="5">
-        <v>0</v>
-      </c>
-      <c r="J24" s="6">
-        <v>0</v>
-      </c>
-      <c r="K24" s="6">
-        <v>0</v>
-      </c>
-      <c r="L24" s="6">
-        <v>0</v>
-      </c>
-      <c r="M24" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24" s="19">
+        <v>0</v>
+      </c>
+      <c r="K24" s="20">
+        <v>0</v>
+      </c>
+      <c r="L24" s="20">
+        <v>0</v>
+      </c>
+      <c r="M24" s="20">
+        <v>0</v>
+      </c>
+      <c r="N24" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="18">
         <v>4</v>
       </c>
       <c r="C25" s="2">
@@ -1687,95 +1785,97 @@
       <c r="D25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="15" t="str">
-        <f>F24</f>
+      <c r="E25" s="17">
+        <v>1</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="15" t="str">
+        <f>G24</f>
         <v>PROF SUP</v>
       </c>
-      <c r="G25" s="8">
+      <c r="H25" s="8">
         <v>5</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="I25" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I25" s="10">
-        <v>0</v>
-      </c>
-      <c r="J25" s="11">
-        <v>0</v>
-      </c>
-      <c r="K25" s="11">
-        <v>0</v>
-      </c>
-      <c r="L25" s="11">
-        <v>0</v>
-      </c>
-      <c r="M25" s="12">
+      <c r="J25" s="22">
+        <v>0</v>
+      </c>
+      <c r="K25" s="23">
+        <v>0</v>
+      </c>
+      <c r="L25" s="23">
+        <v>0</v>
+      </c>
+      <c r="M25" s="23">
+        <v>0</v>
+      </c>
+      <c r="N25" s="24">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A5:M15" xr:uid="{096FA669-5DD0-4A13-82FB-E3FC1F8A4970}"/>
-  <conditionalFormatting sqref="H12:H13 F8 H8:H9 F10 F12">
+  <conditionalFormatting sqref="I12:I13 G8 I8:I9 G10 G12 G18 I18:I19 G20 G22">
     <cfRule type="expression" dxfId="11" priority="12">
-      <formula>$L$8&gt;0</formula>
+      <formula>$M$8&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14:H15">
+  <conditionalFormatting sqref="I14:I15">
     <cfRule type="expression" dxfId="10" priority="11">
-      <formula>$L$8&gt;0</formula>
+      <formula>$M$8&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I14:M15">
+  <conditionalFormatting sqref="J14:N15">
     <cfRule type="expression" dxfId="9" priority="9">
-      <formula>$L$8&gt;0</formula>
+      <formula>$M$8&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F14">
+  <conditionalFormatting sqref="G14">
     <cfRule type="expression" dxfId="8" priority="10">
-      <formula>$L$8&gt;0</formula>
+      <formula>$M$8&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I6:M15">
+  <conditionalFormatting sqref="J6:N15">
     <cfRule type="expression" dxfId="7" priority="8">
-      <formula>$L$8&gt;0</formula>
+      <formula>$M$8&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8:M13">
+  <conditionalFormatting sqref="J8:N13">
     <cfRule type="expression" dxfId="6" priority="7">
-      <formula>$L$8&gt;0</formula>
+      <formula>$M$8&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H22:H23 F18 H18:H19 F20 F22">
+  <conditionalFormatting sqref="I22:I23">
     <cfRule type="expression" dxfId="5" priority="6">
-      <formula>$L$8&gt;0</formula>
+      <formula>$M$8&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24:H25">
+  <conditionalFormatting sqref="I24:I25">
     <cfRule type="expression" dxfId="4" priority="5">
-      <formula>$L$8&gt;0</formula>
+      <formula>$M$8&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I24:M25">
+  <conditionalFormatting sqref="J24:N25">
     <cfRule type="expression" dxfId="3" priority="3">
-      <formula>$L$8&gt;0</formula>
+      <formula>$M$8&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F24">
+  <conditionalFormatting sqref="G24">
     <cfRule type="expression" dxfId="2" priority="4">
-      <formula>$L$8&gt;0</formula>
+      <formula>$M$8&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16:M25">
+  <conditionalFormatting sqref="J16:N25">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$L$8&gt;0</formula>
+      <formula>$M$8&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18:M23">
+  <conditionalFormatting sqref="J18:N23">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$L$8&gt;0</formula>
+      <formula>$M$8&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>